<commit_message>
Update e2e test cases.
</commit_message>
<xml_diff>
--- a/test.e2e.xlsx
+++ b/test.e2e.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baili/go/src/github.com/cybwan/osm.tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55F0D98-7762-6045-9AAB-0B0D56B533BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D9A71B-26D9-4544-960D-8CAC86C7ECC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="-28140" windowWidth="49680" windowHeight="27640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34820" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="测试结果" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">测试结果!$A$1:$M$59</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -668,9 +671,6 @@
   <si>
     <t>e2e_tcp_client_server_test.go</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SimpleClientServer TCP with SMI policies</t>
   </si>
   <si>
     <t>Tests TCP traffic for client pod -&gt; server pod</t>
@@ -904,12 +904,16 @@
     <t>40</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>SimpleClientServer TCP with SMI policies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -990,6 +994,39 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1029,7 +1066,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1087,19 +1124,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1168,23 +1192,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1193,12 +1214,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1213,55 +1228,62 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1270,44 +1292,35 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1593,81 +1606,83 @@
   <dimension ref="A1:N73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" customWidth="1"/>
-    <col min="3" max="3" width="77" customWidth="1"/>
-    <col min="4" max="5" width="9.5" style="17" customWidth="1"/>
-    <col min="6" max="7" width="71.5" customWidth="1"/>
-    <col min="8" max="8" width="107.83203125" customWidth="1"/>
-    <col min="9" max="12" width="12" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="77" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="6" style="14" customWidth="1"/>
+    <col min="6" max="6" width="60" customWidth="1"/>
+    <col min="7" max="7" width="71.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="94" customWidth="1"/>
+    <col min="9" max="12" width="6.83203125" customWidth="1"/>
     <col min="13" max="13" width="29.33203125" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="44"/>
-      <c r="K1" s="43" t="s">
+      <c r="J1" s="49"/>
+      <c r="K1" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="44"/>
+      <c r="L1" s="49"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="4" t="s">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="43" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="27" t="s">
         <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1676,10 +1691,10 @@
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="13">
         <v>2</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="13">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1692,89 +1707,97 @@
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F3,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="CertManagerSimpleClientServer"' make test-e2e</v>
       </c>
-      <c r="I3" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="13" t="s">
+      <c r="I3" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="25">
         <v>1</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="25">
         <v>7</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="42" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="3" t="str">
+      <c r="H4" s="42" t="str">
         <f t="shared" ref="H4:H16" si="0">_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F4,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="Test traffic flowing from client to server with a Kubernetes Service for the Source: HTTP"' make test-e2e</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="13" t="s">
+      <c r="I4" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="52"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="3" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="25">
+        <v>1</v>
+      </c>
+      <c r="E5" s="25">
+        <v>7</v>
+      </c>
+      <c r="F5" s="42" t="s">
         <v>45</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3" t="str">
+      <c r="H5" s="42" t="str">
         <f t="shared" si="0"/>
         <v>E2E_FLAGS='-ginkgo.focus="Test traffic flowing from client to server without a Kubernetes Service for the Source: HTTP"' make test-e2e</v>
       </c>
-      <c r="I5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="13" t="s">
+      <c r="I5" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="53"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="25">
+        <v>1</v>
+      </c>
+      <c r="E6" s="25">
+        <v>7</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>89</v>
       </c>
@@ -1785,33 +1808,33 @@
         <f t="shared" si="0"/>
         <v>E2E_FLAGS='-ginkgo.focus="Test traffic flowing from client to a server with a podIP bind"' make test-e2e</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="13" t="s">
+      <c r="I6" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="54" t="s">
-        <v>202</v>
-      </c>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="18">
         <v>2</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="18">
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1824,33 +1847,33 @@
         <f t="shared" si="0"/>
         <v>E2E_FLAGS='-ginkgo.focus="SimpleClientServer traffic test involving osm-controller restart: HTTP"' make test-e2e</v>
       </c>
-      <c r="I7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="13" t="s">
+      <c r="I7" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="54" t="s">
-        <v>203</v>
-      </c>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="21">
         <v>2</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="21">
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -1863,33 +1886,33 @@
         <f t="shared" si="0"/>
         <v>E2E_FLAGS='-ginkgo.focus="DebugServer"' make test-e2e</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="7" customFormat="1">
-      <c r="A9" s="54" t="s">
+      <c r="I8" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="6" customFormat="1">
+      <c r="A9" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="21">
         <v>1</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="21">
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1902,33 +1925,33 @@
         <f t="shared" si="0"/>
         <v>E2E_FLAGS='-ginkgo.focus="DeploymentsClientServer"' make test-e2e</v>
       </c>
-      <c r="I9" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="7" customFormat="1">
-      <c r="A10" s="51" t="s">
+      <c r="I9" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="6" customFormat="1">
+      <c r="A10" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="24">
         <v>1</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="24">
         <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -1939,25 +1962,29 @@
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F10,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="HTTP egress policy without route matches"' make test-e2e</v>
       </c>
-      <c r="I10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="13" t="s">
+      <c r="I10" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="52"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="24">
+        <v>1</v>
+      </c>
+      <c r="E11" s="24">
+        <v>3</v>
+      </c>
       <c r="F11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1966,25 +1993,29 @@
         <f t="shared" si="0"/>
         <v>E2E_FLAGS='-ginkgo.focus="HTTP egress policy with route match"' make test-e2e</v>
       </c>
-      <c r="I11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="13" t="s">
+      <c r="I11" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="52"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="24">
+        <v>1</v>
+      </c>
+      <c r="E12" s="24">
+        <v>3</v>
+      </c>
       <c r="F12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1993,25 +2024,29 @@
         <f t="shared" si="0"/>
         <v>E2E_FLAGS='-ginkgo.focus="HTTPS egress policy"' make test-e2e</v>
       </c>
-      <c r="I12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="13" t="s">
+      <c r="I12" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="53"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="41">
+        <v>1</v>
+      </c>
+      <c r="E13" s="41">
+        <v>3</v>
+      </c>
       <c r="F13" s="3" t="s">
         <v>22</v>
       </c>
@@ -2022,33 +2057,33 @@
         <f t="shared" si="0"/>
         <v>E2E_FLAGS='-ginkgo.focus="TCP egress policy"' make test-e2e</v>
       </c>
-      <c r="I13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="13" t="s">
+      <c r="I13" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="54" t="s">
-        <v>208</v>
-      </c>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="23">
         <v>1</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="23">
         <v>2</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -2061,33 +2096,33 @@
         <f t="shared" si="0"/>
         <v>E2E_FLAGS='-ginkgo.focus="Egress"' make test-e2e</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L14" s="13" t="s">
+      <c r="I14" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="54" t="s">
-        <v>209</v>
-      </c>
-      <c r="B15" s="22" t="s">
+      <c r="A15" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="21">
         <v>2</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="21">
         <v>3</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -2100,33 +2135,33 @@
         <f t="shared" si="0"/>
         <v>E2E_FLAGS='-ginkgo.focus="Fluent Bit deployment"' make test-e2e</v>
       </c>
-      <c r="I15" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="13" t="s">
+      <c r="I15" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="21">
         <v>2</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="21">
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
@@ -2139,33 +2174,33 @@
         <f t="shared" si="0"/>
         <v>E2E_FLAGS='-ginkgo.focus="Fluent Bit output"' make test-e2e</v>
       </c>
-      <c r="I16" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" s="13" t="s">
+      <c r="I16" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="B17" s="22" t="s">
+      <c r="A17" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="21">
         <v>2</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="21">
         <v>2</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -2178,33 +2213,33 @@
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F17,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="Garbage Collection"' make test-e2e</v>
       </c>
-      <c r="I17" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="7" customFormat="1">
-      <c r="A18" s="54" t="s">
-        <v>188</v>
-      </c>
-      <c r="B18" s="22" t="s">
+      <c r="I17" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="6" customFormat="1">
+      <c r="A18" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="21">
         <v>1</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="21">
         <v>3</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -2217,33 +2252,33 @@
         <f t="shared" ref="H18:H23" si="1">_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F18,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="gRPC insecure traffic origination over HTTP2 with SMI HTTP routes"' make test-e2e</v>
       </c>
-      <c r="I18" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L18" s="13" t="s">
+      <c r="I18" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="54" t="s">
-        <v>189</v>
-      </c>
-      <c r="B19" s="22" t="s">
+      <c r="A19" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="21">
         <v>2</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="21">
         <v>3</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -2256,22 +2291,22 @@
         <f t="shared" si="1"/>
         <v>E2E_FLAGS='-ginkgo.focus="gRPC secure traffic origination over HTTP2 with SMI TCP routes"' make test-e2e</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="K19" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L19" s="13" t="s">
+      <c r="K19" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="54" t="s">
-        <v>190</v>
+      <c r="A20" s="27" t="s">
+        <v>189</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>112</v>
@@ -2279,10 +2314,10 @@
       <c r="C20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="13">
         <v>2</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="13">
         <v>4</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -2295,80 +2330,84 @@
         <f t="shared" si="1"/>
         <v>E2E_FLAGS='-ginkgo.focus="HashivaultSimpleClientServer"' make test-e2e</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="K20" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20" s="9"/>
+      <c r="K20" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1">
-      <c r="A21" s="51" t="s">
-        <v>191</v>
-      </c>
-      <c r="B21" s="27" t="s">
+      <c r="A21" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="25">
         <v>1</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="25">
         <v>4</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="33" t="s">
         <v>35</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="H21" s="27" t="str">
+      <c r="H21" s="33" t="str">
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F21,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="Test health probes can succeed"' make test-e2e</v>
       </c>
-      <c r="I21" s="29" t="s">
+      <c r="I21" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="K21" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="L21" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21" s="8"/>
+      <c r="K21" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" s="7"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="53"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="28"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="25">
+        <v>1</v>
+      </c>
+      <c r="E22" s="25">
+        <v>4</v>
+      </c>
+      <c r="F22" s="35"/>
       <c r="G22" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="8"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="7"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="54" t="s">
-        <v>210</v>
+      <c r="A23" s="27" t="s">
+        <v>209</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>116</v>
@@ -2376,10 +2415,10 @@
       <c r="C23" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="13">
         <v>2</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="13">
         <v>4</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -2392,34 +2431,34 @@
         <f t="shared" si="1"/>
         <v>E2E_FLAGS='-ginkgo.focus="Helm install using default values"' make test-e2e</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="K23" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L23" s="13" t="s">
+      <c r="K23" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="M23" s="8"/>
+      <c r="M23" s="7"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="54" t="s">
-        <v>211</v>
-      </c>
-      <c r="B24" s="19" t="s">
+      <c r="A24" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="18">
         <v>1</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="18">
         <v>2</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -2432,34 +2471,34 @@
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F24,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="Ignore Label"' make test-e2e</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="K24" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L24" s="13" t="s">
+      <c r="K24" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="M24" s="8"/>
+      <c r="M24" s="7"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="54" t="s">
-        <v>192</v>
-      </c>
-      <c r="B25" s="22" t="s">
+      <c r="A25" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="21">
         <v>1</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="21">
         <v>6</v>
       </c>
       <c r="F25" s="3" t="s">
@@ -2472,36 +2511,36 @@
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F25,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="HTTP ingress with IngressBackend"' make test-e2e</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="I25" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="J25" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="K25" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L25" s="13" t="s">
+      <c r="K25" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="M25" s="8" t="s">
-        <v>205</v>
+      <c r="M25" s="7" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="54" t="s">
-        <v>193</v>
-      </c>
-      <c r="B26" s="22" t="s">
+      <c r="A26" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="21">
         <v>2</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="21">
         <v>5</v>
       </c>
       <c r="F26" s="3" t="s">
@@ -2510,38 +2549,38 @@
       <c r="G26" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H26" s="5" t="str">
+      <c r="H26" s="4" t="str">
         <f t="shared" ref="H26:H29" si="2">_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F26,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="When OSM is Installed"' make test-e2e</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="I26" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="J26" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="K26" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L26" s="13" t="s">
+      <c r="K26" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L26" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="M26" s="8"/>
+      <c r="M26" s="7"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="54" t="s">
-        <v>194</v>
-      </c>
-      <c r="B27" s="22" t="s">
+      <c r="A27" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="21">
         <v>2</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="21">
         <v>5</v>
       </c>
       <c r="F27" s="3" t="s">
@@ -2550,38 +2589,38 @@
       <c r="G27" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="H27" s="5" t="str">
+      <c r="H27" s="4" t="str">
         <f t="shared" si="2"/>
         <v>E2E_FLAGS='-ginkgo.focus="Test IP range exclusion"' make test-e2e</v>
       </c>
-      <c r="I27" s="13" t="s">
+      <c r="I27" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="J27" s="13" t="s">
+      <c r="J27" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="K27" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L27" s="13" t="s">
+      <c r="K27" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="M27" s="8"/>
+      <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="54" t="s">
-        <v>195</v>
-      </c>
-      <c r="B28" s="22" t="s">
+      <c r="A28" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="21">
         <v>1</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="21">
         <v>3</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -2590,38 +2629,38 @@
       <c r="G28" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H28" s="5" t="str">
+      <c r="H28" s="4" t="str">
         <f t="shared" si="2"/>
         <v>E2E_FLAGS='-ginkgo.focus="HTTP request rate limiting"' make test-e2e</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="J28" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="K28" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L28" s="13" t="s">
+      <c r="K28" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L28" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="M28" s="8"/>
+      <c r="M28" s="7"/>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="B29" s="22" t="s">
+      <c r="A29" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="21">
         <v>2</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="21">
         <v>6</v>
       </c>
       <c r="F29" s="3" t="s">
@@ -2630,118 +2669,118 @@
       <c r="G29" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H29" s="5" t="str">
+      <c r="H29" s="4" t="str">
         <f t="shared" si="2"/>
         <v>E2E_FLAGS='-ginkgo.focus="Custom WASM metrics between one client pod and one server"' make test-e2e</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="J29" s="14" t="s">
+      <c r="J29" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="K29" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L29" s="13" t="s">
+      <c r="K29" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="M29" s="8" t="s">
-        <v>207</v>
+      <c r="M29" s="7" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:13">
-      <c r="A30" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="B30" s="22" t="s">
+      <c r="A30" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="21">
         <v>2</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="21">
         <v>6</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H30" s="5" t="str">
+      <c r="H30" s="4" t="str">
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F30,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="Multiple service ports"' make test-e2e</v>
       </c>
-      <c r="I30" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K30" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L30" s="13" t="s">
+      <c r="I30" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K30" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L30" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="2" customFormat="1">
-      <c r="A31" s="54" t="s">
-        <v>198</v>
-      </c>
-      <c r="B31" s="22" t="s">
+      <c r="A31" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="23">
         <v>2</v>
       </c>
-      <c r="E31" s="26">
+      <c r="E31" s="23">
         <v>6</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G31" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="H31" s="5" t="str">
+      <c r="H31" s="4" t="str">
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F31,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="Multiple services matching same pod"' make test-e2e</v>
       </c>
-      <c r="I31" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J31" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K31" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L31" s="13" t="s">
+      <c r="I31" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K31" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="54" t="s">
-        <v>199</v>
-      </c>
-      <c r="B32" s="22" t="s">
+      <c r="A32" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="21">
         <v>2</v>
       </c>
-      <c r="E32" s="24">
+      <c r="E32" s="21">
         <v>4</v>
       </c>
       <c r="F32" s="3" t="s">
@@ -2750,37 +2789,37 @@
       <c r="G32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H32" s="5" t="str">
+      <c r="H32" s="4" t="str">
         <f t="shared" ref="H32:H54" si="3">_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F32,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="Test reinstalling OSM in the same namespace with the same mesh name"' make test-e2e</v>
       </c>
-      <c r="I32" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L32" s="13" t="s">
+      <c r="I32" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K32" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L32" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="54" t="s">
-        <v>200</v>
-      </c>
-      <c r="B33" s="22" t="s">
+      <c r="A33" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="24">
+      <c r="D33" s="21">
         <v>1</v>
       </c>
-      <c r="E33" s="24">
+      <c r="E33" s="21">
         <v>2</v>
       </c>
       <c r="F33" s="3" t="s">
@@ -2789,171 +2828,179 @@
       <c r="G33" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H33" s="5" t="str">
+      <c r="H33" s="4" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="PermissiveToSmiSwitching"' make test-e2e</v>
       </c>
-      <c r="I33" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J33" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K33" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L33" s="13" t="s">
+      <c r="I33" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K33" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L33" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34" s="51" t="s">
-        <v>201</v>
-      </c>
-      <c r="B34" s="35" t="s">
+      <c r="A34" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="B34" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="D34" s="33">
+      <c r="D34" s="24">
         <v>1</v>
       </c>
-      <c r="E34" s="33">
+      <c r="E34" s="24">
         <v>7</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G34" s="3"/>
-      <c r="H34" s="5" t="str">
+      <c r="H34" s="4" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="Permissive mode HTTP test with a Kubernetes Service for the Source"' make test-e2e</v>
       </c>
-      <c r="I34" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L34" s="13" t="s">
+      <c r="I34" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J34" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K34" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L34" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="53"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="24">
+        <v>1</v>
+      </c>
+      <c r="E35" s="24">
+        <v>7</v>
+      </c>
       <c r="F35" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="H35" s="5" t="str">
+      <c r="H35" s="4" t="str">
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F35,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="Permissive mode HTTP test without a Kubernetes Service for the Source"' make test-e2e</v>
       </c>
-      <c r="I35" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J35" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K35" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L35" s="13" t="s">
+      <c r="I35" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K35" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="51" t="s">
-        <v>212</v>
-      </c>
-      <c r="B36" s="35" t="s">
+      <c r="A36" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="B36" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="D36" s="33">
+      <c r="D36" s="24">
         <v>2</v>
       </c>
-      <c r="E36" s="33">
+      <c r="E36" s="24">
         <v>7</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="H36" s="5" t="str">
+        <v>183</v>
+      </c>
+      <c r="H36" s="4" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="Test global port exclusion"' make test-e2e</v>
       </c>
-      <c r="I36" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L36" s="13" t="s">
+      <c r="I36" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K36" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L36" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="53"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="41">
+        <v>2</v>
+      </c>
+      <c r="E37" s="41">
+        <v>7</v>
+      </c>
       <c r="F37" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="Test pod level port exclusion"' make test-e2e</v>
       </c>
-      <c r="I37" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J37" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K37" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L37" s="13" t="s">
+      <c r="I37" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K37" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L37" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="54" t="s">
-        <v>213</v>
-      </c>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="B38" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="24">
+      <c r="D38" s="41">
         <v>2</v>
       </c>
-      <c r="E38" s="24">
+      <c r="E38" s="41">
         <v>8</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -2966,203 +3013,219 @@
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="proxy resources"' make test-e2e</v>
       </c>
-      <c r="I38" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K38" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L38" s="13" t="s">
+      <c r="I38" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J38" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K38" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L38" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="51" t="s">
-        <v>214</v>
-      </c>
-      <c r="B39" s="27" t="s">
+      <c r="A39" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B39" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="33">
+      <c r="D39" s="24">
         <v>2</v>
       </c>
-      <c r="E39" s="33">
+      <c r="E39" s="24">
         <v>9</v>
       </c>
-      <c r="F39" s="27" t="s">
+      <c r="F39" s="33" t="s">
         <v>48</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="H39" s="27" t="str">
+      <c r="H39" s="33" t="str">
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F39,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="Enable Reconciler"' make test-e2e</v>
       </c>
-      <c r="I39" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="K39" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="L39" s="29" t="s">
+      <c r="I39" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="L39" s="45" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="52"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="31"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="24">
+        <v>2</v>
+      </c>
+      <c r="E40" s="24">
+        <v>9</v>
+      </c>
+      <c r="F40" s="34"/>
       <c r="G40" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="H40" s="31"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="48"/>
+      <c r="L40" s="48"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="53"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="5" t="s">
+      <c r="A41" s="29"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="24">
+        <v>2</v>
+      </c>
+      <c r="E41" s="24">
+        <v>9</v>
+      </c>
+      <c r="F41" s="35"/>
+      <c r="G41" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="H41" s="28"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="30"/>
-      <c r="L41" s="30"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="51" t="s">
-        <v>215</v>
+      <c r="A42" s="28" t="s">
+        <v>214</v>
       </c>
       <c r="B42" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="D42" s="33">
+      <c r="D42" s="24">
         <v>2</v>
       </c>
-      <c r="E42" s="33">
+      <c r="E42" s="24">
         <v>4</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G42" s="4" t="s">
         <v>157</v>
       </c>
       <c r="H42" s="3" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="Retry policy disabled"' make test-e2e</v>
       </c>
-      <c r="I42" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J42" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K42" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L42" s="13" t="s">
+      <c r="I42" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K42" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L42" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="53"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="40"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="5" t="s">
+      <c r="C43" s="38"/>
+      <c r="D43" s="24">
+        <v>2</v>
+      </c>
+      <c r="E43" s="24">
+        <v>4</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G43" s="4" t="s">
         <v>160</v>
       </c>
       <c r="H43" s="3" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="Retry policy enabled"' make test-e2e</v>
       </c>
-      <c r="I43" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J43" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K43" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L43" s="13" t="s">
+      <c r="I43" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J43" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K43" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L43" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="51" t="s">
-        <v>216</v>
-      </c>
-      <c r="B44" s="27" t="s">
+      <c r="A44" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B44" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D44" s="33">
+      <c r="D44" s="24">
         <v>1</v>
       </c>
-      <c r="E44" s="33">
+      <c r="E44" s="24">
         <v>8</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="5" t="s">
+      <c r="G44" s="4" t="s">
         <v>161</v>
       </c>
       <c r="H44" s="3" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="SMI Traffic Target is not in the same namespace as the destination"' make test-e2e</v>
       </c>
-      <c r="I44" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J44" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K44" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L44" s="13" t="s">
+      <c r="I44" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J44" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K44" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L44" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="53"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="41">
+        <v>1</v>
+      </c>
+      <c r="E45" s="41">
+        <v>8</v>
+      </c>
       <c r="F45" s="3" t="s">
         <v>162</v>
       </c>
@@ -3173,35 +3236,35 @@
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="SMI TrafficTarget is set up properly"' make test-e2e</v>
       </c>
-      <c r="I45" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J45" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K45" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L45" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
+      <c r="I45" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J45" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K45" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L45" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="B46" s="15" t="s">
+      <c r="A46" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="B46" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="D46" s="24">
+      <c r="D46" s="41">
         <v>1</v>
       </c>
-      <c r="E46" s="24">
+      <c r="E46" s="41">
         <v>9</v>
       </c>
       <c r="F46" s="3" t="s">
@@ -3214,147 +3277,151 @@
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F46,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="Statefulsets"' make test-e2e</v>
       </c>
-      <c r="I46" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J46" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K46" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L46" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
+      <c r="I46" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J46" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K46" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L46" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="51" t="s">
-        <v>218</v>
-      </c>
-      <c r="B47" s="27" t="s">
+      <c r="A47" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="C47" s="35" t="s">
+      <c r="C47" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="33">
+      <c r="D47" s="24">
         <v>1</v>
       </c>
-      <c r="E47" s="33">
+      <c r="E47" s="24">
         <v>8</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>168</v>
+        <v>225</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="SimpleClientServer TCP with SMI policies"' make test-e2e</v>
       </c>
-      <c r="I47" s="14" t="s">
+      <c r="I47" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="J47" s="14" t="s">
+      <c r="J47" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="K47" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L47" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M47" s="50" t="s">
-        <v>206</v>
+      <c r="K47" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L47" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="M47" s="26" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:14" s="2" customFormat="1">
-      <c r="A48" s="53"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="6" t="s">
+      <c r="A48" s="29"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="41">
+        <v>1</v>
+      </c>
+      <c r="E48" s="41">
         <v>8</v>
       </c>
-      <c r="G48" s="6" t="s">
-        <v>169</v>
+      <c r="F48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="H48" s="3" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="SimpleClientServer TCP in permissive mode"' make test-e2e</v>
       </c>
-      <c r="I48" s="14" t="s">
+      <c r="I48" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="J48" s="14" t="s">
+      <c r="J48" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="K48" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L48" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M48" s="50" t="s">
-        <v>206</v>
-      </c>
-      <c r="N48" s="11"/>
+      <c r="K48" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L48" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="M48" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="N48" s="10"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="B49" s="15" t="s">
+      <c r="A49" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="C49" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="D49" s="24">
+      <c r="D49" s="41">
         <v>1</v>
       </c>
-      <c r="E49" s="24">
+      <c r="E49" s="41">
         <v>9</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H49" s="3" t="str">
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F49,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="SimpleClientServer egress TCP"' make test-e2e</v>
       </c>
-      <c r="I49" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J49" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K49" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L49" s="13" t="s">
+      <c r="I49" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J49" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K49" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L49" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="54" t="s">
-        <v>220</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C50" s="23" t="s">
+      <c r="A50" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C50" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D50" s="24">
+      <c r="D50" s="21">
         <v>1</v>
       </c>
-      <c r="E50" s="24">
+      <c r="E50" s="21">
         <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
@@ -3367,141 +3434,145 @@
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="TCP server-first traffic"' make test-e2e</v>
       </c>
-      <c r="I50" s="14" t="s">
+      <c r="I50" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="J50" s="14" t="s">
+      <c r="J50" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="K50" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L50" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M50" s="50" t="s">
-        <v>206</v>
+      <c r="K50" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L50" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="M50" s="26" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:13">
-      <c r="A51" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="B51" s="27" t="s">
+      <c r="A51" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="B51" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="C51" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="C51" s="35" t="s">
+      <c r="D51" s="24">
+        <v>1</v>
+      </c>
+      <c r="E51" s="24">
+        <v>9</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="D51" s="33">
-        <v>1</v>
-      </c>
-      <c r="E51" s="33">
-        <v>9</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="HTTP recursive traffic splitting with SMI"' make test-e2e</v>
       </c>
-      <c r="I51" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J51" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K51" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L51" s="13" t="s">
+      <c r="I51" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J51" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K51" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L51" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="53"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
+      <c r="A52" s="29"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="41">
+        <v>1</v>
+      </c>
+      <c r="E52" s="41">
+        <v>9</v>
+      </c>
       <c r="F52" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="H52" s="3" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="TCP recursive traffic splitting with SMI"' make test-e2e</v>
       </c>
-      <c r="I52" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J52" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K52" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L52" s="13" t="s">
+      <c r="I52" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J52" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K52" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L52" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" s="54" t="s">
-        <v>222</v>
-      </c>
-      <c r="B53" s="15" t="s">
+      <c r="A53" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="B53" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C53" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="D53" s="24">
+      <c r="C53" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" s="41">
         <v>1</v>
       </c>
-      <c r="E53" s="24">
+      <c r="E53" s="41">
         <v>9</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H53" s="3" t="str">
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="ClientServerTrafficSplitSameSA"' make test-e2e</v>
       </c>
-      <c r="I53" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J53" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K53" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L53" s="13" t="s">
+      <c r="I53" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J53" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K53" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L53" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="51" t="s">
-        <v>223</v>
-      </c>
-      <c r="B54" s="27" t="s">
+      <c r="A54" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="C54" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="D54" s="33">
+      <c r="D54" s="24">
         <v>1</v>
       </c>
-      <c r="E54" s="33">
+      <c r="E54" s="24">
         <v>5</v>
       </c>
       <c r="F54" s="3" t="s">
@@ -3512,25 +3583,29 @@
         <f t="shared" si="3"/>
         <v>E2E_FLAGS='-ginkgo.focus="HTTP traffic splitting with SMI"' make test-e2e</v>
       </c>
-      <c r="I54" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J54" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K54" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L54" s="13" t="s">
+      <c r="I54" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J54" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K54" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L54" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:13">
-      <c r="A55" s="52"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="24">
+        <v>1</v>
+      </c>
+      <c r="E55" s="24">
+        <v>5</v>
+      </c>
       <c r="F55" s="3" t="s">
         <v>30</v>
       </c>
@@ -3539,62 +3614,66 @@
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F55,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="TCP traffic splitting with SMI"' make test-e2e</v>
       </c>
-      <c r="I55" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J55" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K55" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L55" s="13" t="s">
+      <c r="I55" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J55" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K55" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L55" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="53"/>
-      <c r="B56" s="28"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
+      <c r="A56" s="29"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="41">
+        <v>1</v>
+      </c>
+      <c r="E56" s="41">
+        <v>5</v>
+      </c>
       <c r="F56" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H56" s="3" t="str">
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F56,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="HTTP traffic splitting with Permissive mode"' make test-e2e</v>
       </c>
-      <c r="I56" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J56" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K56" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L56" s="13" t="s">
+      <c r="I56" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J56" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K56" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L56" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="54" t="s">
-        <v>224</v>
-      </c>
-      <c r="B57" s="15" t="s">
+      <c r="A57" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="B57" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="23" t="s">
+      <c r="C57" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="24">
+      <c r="D57" s="21">
         <v>2</v>
       </c>
-      <c r="E57" s="24">
+      <c r="E57" s="21">
         <v>10</v>
       </c>
       <c r="F57" s="3" t="s">
@@ -3607,351 +3686,335 @@
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F57,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="Upgrade from latest"' make test-e2e</v>
       </c>
-      <c r="I57" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J57" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K57" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L57" s="13" t="s">
+      <c r="I57" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J57" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K57" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L57" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="51" t="s">
-        <v>225</v>
-      </c>
-      <c r="B58" s="27" t="s">
+      <c r="A58" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B58" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="35" t="s">
+      <c r="C58" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="33">
+      <c r="D58" s="41">
         <v>1</v>
       </c>
-      <c r="E58" s="33">
+      <c r="E58" s="41">
         <v>8</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H58" s="3" t="str">
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F58,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="With SMI Traffic Target validation enabled "' make test-e2e</v>
       </c>
-      <c r="I58" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J58" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K58" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L58" s="13" t="s">
+      <c r="I58" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J58" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K58" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L58" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="53"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
+      <c r="A59" s="29"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="41">
+        <v>1</v>
+      </c>
+      <c r="E59" s="41">
+        <v>8</v>
+      </c>
       <c r="F59" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H59" s="3" t="str">
         <f>_xlfn.CONCAT("E2E_FLAGS='-ginkgo.focus=""",F59,"""' make test-e2e")</f>
         <v>E2E_FLAGS='-ginkgo.focus="With SMI validation disabled"' make test-e2e</v>
       </c>
-      <c r="I59" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J59" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K59" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L59" s="13" t="s">
+      <c r="I59" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J59" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K59" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L59" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="14" customHeight="1">
-      <c r="A61" s="47" t="s">
-        <v>204</v>
-      </c>
-      <c r="B61" s="48"/>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="48"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="48"/>
-      <c r="H61" s="48"/>
-      <c r="I61" s="48"/>
-      <c r="J61" s="48"/>
-      <c r="K61" s="12"/>
-      <c r="L61" s="12"/>
+      <c r="A61" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="32"/>
+      <c r="I61" s="32"/>
+      <c r="J61" s="32"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="11"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="47"/>
-      <c r="B62" s="48"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="48"/>
-      <c r="E62" s="48"/>
-      <c r="F62" s="48"/>
-      <c r="G62" s="48"/>
-      <c r="H62" s="48"/>
-      <c r="I62" s="48"/>
-      <c r="J62" s="48"/>
-      <c r="K62" s="12"/>
-      <c r="L62" s="12"/>
+      <c r="A62" s="31"/>
+      <c r="B62" s="32"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="32"/>
+      <c r="I62" s="32"/>
+      <c r="J62" s="32"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="11"/>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" s="47"/>
-      <c r="B63" s="48"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
-      <c r="E63" s="48"/>
-      <c r="F63" s="48"/>
-      <c r="G63" s="48"/>
-      <c r="H63" s="48"/>
-      <c r="I63" s="48"/>
-      <c r="J63" s="48"/>
-      <c r="K63" s="12"/>
-      <c r="L63" s="12"/>
+      <c r="A63" s="31"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="11"/>
+      <c r="L63" s="11"/>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64" s="47"/>
-      <c r="B64" s="48"/>
-      <c r="C64" s="48"/>
-      <c r="D64" s="48"/>
-      <c r="E64" s="48"/>
-      <c r="F64" s="48"/>
-      <c r="G64" s="48"/>
-      <c r="H64" s="48"/>
-      <c r="I64" s="48"/>
-      <c r="J64" s="48"/>
-      <c r="K64" s="12"/>
-      <c r="L64" s="12"/>
+      <c r="A64" s="31"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="47"/>
-      <c r="B65" s="48"/>
-      <c r="C65" s="48"/>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="48"/>
-      <c r="G65" s="48"/>
-      <c r="H65" s="48"/>
-      <c r="I65" s="48"/>
-      <c r="J65" s="48"/>
-      <c r="K65" s="12"/>
-      <c r="L65" s="12"/>
+      <c r="A65" s="31"/>
+      <c r="B65" s="32"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="32"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="32"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="11"/>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="47"/>
-      <c r="B66" s="48"/>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="48"/>
-      <c r="I66" s="48"/>
-      <c r="J66" s="48"/>
-      <c r="K66" s="12"/>
-      <c r="L66" s="12"/>
+      <c r="A66" s="31"/>
+      <c r="B66" s="32"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="32"/>
+      <c r="G66" s="32"/>
+      <c r="H66" s="32"/>
+      <c r="I66" s="32"/>
+      <c r="J66" s="32"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="11"/>
     </row>
     <row r="67" spans="1:12">
-      <c r="A67" s="47"/>
-      <c r="B67" s="48"/>
-      <c r="C67" s="48"/>
-      <c r="D67" s="48"/>
-      <c r="E67" s="48"/>
-      <c r="F67" s="48"/>
-      <c r="G67" s="48"/>
-      <c r="H67" s="48"/>
-      <c r="I67" s="48"/>
-      <c r="J67" s="48"/>
-      <c r="K67" s="12"/>
-      <c r="L67" s="12"/>
+      <c r="A67" s="31"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="32"/>
+      <c r="G67" s="32"/>
+      <c r="H67" s="32"/>
+      <c r="I67" s="32"/>
+      <c r="J67" s="32"/>
+      <c r="K67" s="11"/>
+      <c r="L67" s="11"/>
     </row>
     <row r="68" spans="1:12">
-      <c r="A68" s="47"/>
-      <c r="B68" s="48"/>
-      <c r="C68" s="48"/>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="48"/>
-      <c r="G68" s="48"/>
-      <c r="H68" s="48"/>
-      <c r="I68" s="48"/>
-      <c r="J68" s="48"/>
-      <c r="K68" s="12"/>
-      <c r="L68" s="12"/>
+      <c r="A68" s="31"/>
+      <c r="B68" s="32"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="32"/>
+      <c r="H68" s="32"/>
+      <c r="I68" s="32"/>
+      <c r="J68" s="32"/>
+      <c r="K68" s="11"/>
+      <c r="L68" s="11"/>
     </row>
     <row r="69" spans="1:12">
-      <c r="A69" s="47"/>
-      <c r="B69" s="48"/>
-      <c r="C69" s="48"/>
-      <c r="D69" s="48"/>
-      <c r="E69" s="48"/>
-      <c r="F69" s="48"/>
-      <c r="G69" s="48"/>
-      <c r="H69" s="48"/>
-      <c r="I69" s="48"/>
-      <c r="J69" s="48"/>
-      <c r="K69" s="12"/>
-      <c r="L69" s="12"/>
+      <c r="A69" s="31"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="32"/>
+      <c r="H69" s="32"/>
+      <c r="I69" s="32"/>
+      <c r="J69" s="32"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="47"/>
-      <c r="B70" s="48"/>
-      <c r="C70" s="48"/>
-      <c r="D70" s="48"/>
-      <c r="E70" s="48"/>
-      <c r="F70" s="48"/>
-      <c r="G70" s="48"/>
-      <c r="H70" s="48"/>
-      <c r="I70" s="48"/>
-      <c r="J70" s="48"/>
-      <c r="K70" s="12"/>
-      <c r="L70" s="12"/>
+      <c r="A70" s="31"/>
+      <c r="B70" s="32"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="32"/>
+      <c r="G70" s="32"/>
+      <c r="H70" s="32"/>
+      <c r="I70" s="32"/>
+      <c r="J70" s="32"/>
+      <c r="K70" s="11"/>
+      <c r="L70" s="11"/>
     </row>
     <row r="71" spans="1:12">
-      <c r="A71" s="47"/>
-      <c r="B71" s="48"/>
-      <c r="C71" s="48"/>
-      <c r="D71" s="48"/>
-      <c r="E71" s="48"/>
-      <c r="F71" s="48"/>
-      <c r="G71" s="48"/>
-      <c r="H71" s="48"/>
-      <c r="I71" s="48"/>
-      <c r="J71" s="48"/>
-      <c r="K71" s="12"/>
-      <c r="L71" s="12"/>
+      <c r="A71" s="31"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="32"/>
+      <c r="G71" s="32"/>
+      <c r="H71" s="32"/>
+      <c r="I71" s="32"/>
+      <c r="J71" s="32"/>
+      <c r="K71" s="11"/>
+      <c r="L71" s="11"/>
     </row>
     <row r="72" spans="1:12">
-      <c r="A72" s="47"/>
-      <c r="B72" s="48"/>
-      <c r="C72" s="48"/>
-      <c r="D72" s="48"/>
-      <c r="E72" s="48"/>
-      <c r="F72" s="48"/>
-      <c r="G72" s="48"/>
-      <c r="H72" s="48"/>
-      <c r="I72" s="48"/>
-      <c r="J72" s="48"/>
-      <c r="K72" s="12"/>
-      <c r="L72" s="12"/>
+      <c r="A72" s="31"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="32"/>
+      <c r="G72" s="32"/>
+      <c r="H72" s="32"/>
+      <c r="I72" s="32"/>
+      <c r="J72" s="32"/>
+      <c r="K72" s="11"/>
+      <c r="L72" s="11"/>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="10"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="83">
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A61:J72"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A10:A13"/>
+  <autoFilter ref="A1:M59" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="8" showButton="0"/>
+    <filterColumn colId="10" showButton="0"/>
+  </autoFilter>
+  <mergeCells count="59">
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="I39:I41"/>
+    <mergeCell ref="J39:J41"/>
+    <mergeCell ref="K39:K41"/>
+    <mergeCell ref="L39:L41"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B34:B35"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="I39:I41"/>
-    <mergeCell ref="J39:J41"/>
-    <mergeCell ref="K39:K41"/>
-    <mergeCell ref="L39:L41"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="A61:J72"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A58:A59"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>